<commit_message>
modified:   anuncios.xlsx modified:   models_api/api_max.py modified:   models_excel/core.py modified:   view/interface.py renamed:    ~$plan.xlsx -> ~$anuncios.xlsx
</commit_message>
<xml_diff>
--- a/anuncios.xlsx
+++ b/anuncios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,15 +456,20 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>descricao</t>
+          <t>aplicacao completa</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>aplicacao simplificada</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>posicao</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>lado</t>
         </is>
@@ -493,16 +498,36 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2062
+          <t>Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2062
 Marca: CONTROIL
 Código Produto: C-2062
 Compatível com os veículos:
-FORD F-4000 (4 BTAA 8V)/(SERIE 10 / X10)/(SERIE 229) 1992-1998 F-1000 2.5 8V/3.9 8V/4.9 12V 1992-1998
-            </t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+FORD F-1000 L 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
+FORD F-1000 LWB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
+FORD F-4000 - 1984 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 85cv
+FORD F-1000 L 1992 a 1995 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 91cv
+FORD F-4000 - 1993 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
+FORD F-4000 - 1996 a 2008 - Motor: 4 BTAA 8V 3917cc 3.9 L 8V SOHV L4 141cv
+FORD F-1000 4X4 1992 a 1995 - Motor: SERIE 229 3922cc 3.9 L 8V SOHV L4 122cv
+FORD F-1000 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+FORD F-1000 L 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+FORD F-1000 XLT 1996 a 1998 - Motor: HS4 2495cc 2.5 L 8V SOHC L4 116cv
+FORD F-1000 S.CAB 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+FORD F-4000 - 1996 a 1998 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+FORD F-1000 S CAB 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
+FORD F-1000 S.CAB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2062
+Marca: CONTROIL
+Código Produto: C-2062
+Compatível com os veículos:FORD F-4000 (4 BTAA 8V)/(SERIE 10 / X10)/(SERIE 229) 1992-1998 F-1000 2.5 8V/3.9 8V/4.9 12V 1992-1998</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -527,16 +552,40 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2044
+          <t>Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2044
 Marca: CONTROIL
 Código Produto: C-2044
 Compatível com os veículos:
-CHEVROLET D-20 3.9 8V 1985-1992 C-20 4.1 12V 1985-1995 BONANZA 4.1 12V 1989-1995 A-20 4.1 12V 1985-1995 AGRALE 1800 (Q20B)/(SERIE 229) 1988-1998
-            </t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+CHEVROLET BONANZA CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET BONANZA CUSTOM S LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET C-20 4X4 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+CHEVROLET A-20 CUSTOM S 1985 a 1997 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET A-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET D-20 D 20 1985 a 1991 - Motor: Q20B 3871cc 3.9 L 8V SOHC L4 86,4cv
+CHEVROLET A-20 CUSTOM LUXE 1991 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET D-20 CUSTOM LUXE 1991 a 1992 - Motor: Q20B 3871cc 3.9 L 8V SOHC L4 86,4cv
+CHEVROLET A-20 CUSTOM S 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+AGRALE 1800 D 1988 a 1996 - Motor: Q20B 3871cc 3.9 L 8V SOHV L4 86,4cv
+CHEVROLET C-20 STD 1994 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+CHEVROLET A-20 CUSTOM S CAB DUP 1985 a 1996 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET C-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+AGRALE 1800 D 1988 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 88cv
+CHEVROLET D-20 CUSTOM S 1988 a 1991 - Motor: Q20B 3871cc 3.9 L 8V SOHC L4 86,4cv
+CHEVROLET BONANZA CUSTOM S 1989 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET BONANZA CUSTOM S 1989 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET C-20 - 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2044
+Marca: CONTROIL
+Código Produto: C-2044
+Compatível com os veículos:CHEVROLET D-20 3.9 8V 1985-1992 C-20 4.1 12V 1985-1995 BONANZA 4.1 12V 1989-1995 A-20 4.1 12V 1985-1995 AGRALE 1800 (Q20B)/(SERIE 229) 1988-1998</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -561,16 +610,29 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3308
+          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3308
 Marca: CONTROIL
 Código Produto: C-3308
 Compatível com os veículos:
-FORD F-4000 (D 226-4) 1979-1983 F-400 (272) 1975-1977 AGRALE 1600 (-)/(SERIE 229) 1985-1989 1800 (Q20B)/(SERIE 229) 1988-1989
-            </t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr">
+AGRALE 1600 A 1986 a 1994 - Motor: - 2470cc 2.5 L 8V SOHC L4 75cv
+AGRALE 1800 D 1988 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 88cv
+AGRALE 1800 D 1988 a 1996 - Motor: Q20B 3871cc 3.9 L 8V SOHV L4 86,4cv
+AGRALE 1600 D 1986 a 1989 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 88cv
+FORD F-400 - 1975 a 1977 - Motor: 272 4457cc 4.5 L 16V OHC V8 165cv
+FORD F-4000 - 1978 a 1986 - Motor: D 226-4 4160cc 4.2 L 8V SOHV L4 86cv
+AGRALE 1600 D 1986 a 1991 - Motor: SERIE 229 2942cc 3.0 L 6V SOHV L3 62cv</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3308
+Marca: CONTROIL
+Código Produto: C-3308
+Compatível com os veículos:FORD F-4000 (D 226-4) 1979-1983 F-400 (272) 1975-1977 AGRALE 1600 (-)/(SERIE 229) 1985-1989 1800 (Q20B)/(SERIE 229) 1988-1989</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Direito</t>
         </is>
@@ -599,16 +661,27 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t xml:space="preserve">Produto: CILINDRO DE RODA CONTROIL - C-3334
+          <t>Produto: CILINDRO DE RODA CONTROIL - C-3334
 Marca: CONTROIL
 Código Produto: C-3334
 Compatível com os veículos:
-MERCEDES BENZ L 709 (OM 364) 1988-1996 912 (OM 364 A) 1988-2003 710 (OM 364 A) 1995-2002
-            </t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
+MERCEDES BENZ 912 - 1988 a 1996 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 122cv
+MERCEDES BENZ L 709 - 1988 a 1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 90cv
+MERCEDES BENZ L 709 - 1990 a 1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 115cv
+MERCEDES BENZ L 709 37/42 1988 a 1996 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 90cv
+MERCEDES BENZ 710 - 1995 a 1997 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 110cv</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Produto: CILINDRO DE RODA CONTROIL - C-3334
+Marca: CONTROIL
+Código Produto: C-3334
+Compatível com os veículos:MERCEDES BENZ L 709 (OM 364) 1988-1996 912 (OM 364 A) 1988-2003 710 (OM 364 A) 1995-2002</t>
+        </is>
+      </c>
       <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -633,16 +706,26 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3377
+          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3377
 Marca: CONTROIL
 Código Produto: C-3377
 Compatível com os veículos:
-FORD F-1000 3.9 8V 1979-1992
-            </t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr">
+FORD F-1000 L 1981 a 1986 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
+FORD F-1000 L 1979 a 1979 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
+FORD F-1000 L 1979 a 1991 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
+FORD F-1000 L 1980 a 1981 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3377
+Marca: CONTROIL
+Código Produto: C-3377
+Compatível com os veículos:FORD F-1000 3.9 8V 1979-1992</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
         <is>
           <t>Direito</t>
         </is>
@@ -671,16 +754,75 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Produto: REPARO DO CILINDRO MESTRE CONTROIL - C-1125
+          <t>Produto: REPARO DO CILINDRO MESTRE CONTROIL - C-1125
 Marca: CONTROIL
 Código Produto: C-1125
 Compatível com os veículos:
-CHEVROLET D-20 4.0 8V 1993-1996 VERANEIO 4.1 12V 1993-1995 C-20 4.1 12V 1993-1996 FORD F-4000 (4 BTAA 8V)/(SERIE 10 / X10)/(SERIE 229) 1992-1998 F-1000 2.5 8V/3.9 8V/4.9 12V 1992-1998
-            </t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
+CHEVROLET C-20 - 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+CHEVROLET D-20 CUSTOM S TURBO 1992 a 1996 - Motor: S4T 3998cc 4.0 L 8V SOHC L4 120cv
+CHEVROLET VERANEIO LUXE 1993 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET VERANEIO CUSTOM LUXE 1992 a 1993 - Motor: MAXION 3990cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET D-20 CUSTOM LUXE TURBO 1992 a 1996 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+FORD F-4000 - 1984 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 85cv
+CHEVROLET D-20 CHAMP TB 1994 a 1994 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+CHEVROLET D-20 CUSTOM S TURBO 1992 a 1995 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+CHEVROLET D-20 CHAMP 1994 a 1994 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+CHEVROLET C-20 STD 1996 a 1999 - Motor: POWERTECH 4095cc 4.1 L 12V SOHC L6 225cv
+CHEVROLET C-20 4X4 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+CHEVROLET A-20 CUSTOM S 1985 a 1997 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET VERANEIO - 1966 a 1988 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET VERANEIO CUSTOM S 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+FORD F-1000 S CAB 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
+FORD F-4000 - 1993 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
+CHEVROLET A-20 CUSTOM S 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+FORD F-1000 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+CHEVROLET D-20 CUSTOM LUXE TURBO 1996 a 1996 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+CHEVROLET A-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET C-20 CUSTOM LUXE 1996 a 1996 - Motor: POWERTECH 4095cc 4.1 L 12V SOHC L6 225cv
+CHEVROLET C-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+CHEVROLET D-20 LX 1994 a 1998 - Motor: S4T 3998cc 4.0 L 8V SOHC L4 120cv
+CHEVROLET D-20 CUSTOM LUXE 1992 a 1996 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET BONANZA CUSTOM L TB 1992 a 1994 - Motor: S4T 4000cc 4.0 L 8V SOHC L4 120cv
+FORD F-1000 L 1992 a 1995 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 91cv
+FORD F-1000 XLT 1996 a 1998 - Motor: HS4 2495cc 2.5 L 8V SOHC L4 116cv
+CHEVROLET A-20 CUSTOM LUXE 1991 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET D-20 CONQUEST TURBO 1992 a 1995 - Motor: S4T PLUS 3998cc 4.0 L 8V OHV L4 150cv
+FORD F-1000 LWB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
+CHEVROLET BONANZA CUSTOM S 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+FORD F-1000 S.CAB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
+FORD F-1000 S.CAB 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+CHEVROLET BONANZA CUSTOM S 1989 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET BONANZA CUSTOM S TB 1992 a 1995 - Motor: S4T 4000cc 4.0 L 8V SOHC L4 120cv
+CHEVROLET VERANEIO CUSTOM 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET D-20 CONQUEST 1992 a 1994 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET VERANEIO CUSTOM LUXE 1993 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET BONANZA CUSTOM LUXE 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+FORD F-1000 L 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+CHEVROLET VERANEIO - 1983 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+FORD F-4000 - 1996 a 2008 - Motor: 4 BTAA 8V 3917cc 3.9 L 8V SOHV L4 141cv
+CHEVROLET A-20 CUSTOM S CAB DUP 1985 a 1996 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+FORD F-1000 L 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
+CHEVROLET C-20 STD 1994 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+FORD F-4000 - 1996 a 1998 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+FORD F-1000 4X4 1992 a 1995 - Motor: SERIE 229 3922cc 3.9 L 8V SOHV L4 122cv
+CHEVROLET BONANZA CUSTOM S 1989 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET D-20 CUSTOM S 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET BONANZA CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET VERANEIO CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET BONANZA CUSTOM S LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET VERANEIO CUSTOM LUXE 1991 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO CILINDRO MESTRE CONTROIL - C-1125
+Marca: CONTROIL
+Código Produto: C-1125
+Compatível com os veículos:CHEVROLET D-20 4.0 8V 1993-1996 VERANEIO 4.1 12V 1993-1995 C-20 4.1 12V 1993-1996 FORD F-4000 (4 BTAA 8V)/(SERIE 10 / X10)/(SERIE 229) 1992-1998 F-1000 2.5 8V/3.9 8V/4.9 12V 1992-1998</t>
+        </is>
+      </c>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -705,16 +847,23 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t xml:space="preserve">Produto: REPARO DO CILINDRO DE RODA CONTROIL - C-1478
+          <t>Produto: REPARO DO CILINDRO DE RODA CONTROIL - C-1478
 Marca: CONTROIL
 Código Produto: C-1478
 Compatível com os veículos:
-MERCEDES BENZ L 1519 (OM 355/5) 1973-1987
-            </t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr"/>
+MERCEDES BENZ L 1519 - 1972 a 2023 - Motor: OM 355/5 9650cc 9.7 L 10V SOHV L5 192cv</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO CILINDRO DE RODA CONTROIL - C-1478
+Marca: CONTROIL
+Código Produto: C-1478
+Compatível com os veículos:MERCEDES BENZ L 1519 (OM 355/5) 1973-1987</t>
+        </is>
+      </c>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modified:   anuncios.xlsx modified:   models_api/api_max.py modified:   models_excel/core.py modified:   models_excel/padroes_substituir_nomes_anuncios.py modified:   plan.xlsx new file:   tabledata_20250620_143834.csv modified:   teste.py modified:   view/interface.py
</commit_message>
<xml_diff>
--- a/anuncios.xlsx
+++ b/anuncios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,392 +478,93 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>C-2062</t>
+          <t>HG 30873</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cilindro Mestre De Freio Compatível Ford F-4000 (4 Btaa 8V)/(Serie 10 / X10)/(Serie 229) 1992-1998 Controil C-2062</t>
+          <t>Amortecedor P/ Suspensão Compatível Chevrolet Astra 1.8 8V/2.0 8V/2.4 16V 1998-2011 Traseiro Direito / Esquerdo Nakata Hg 30873</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Cilindro Mestre Freio Compatível F-4000 1992-1998</t>
+          <t>Amortecedor P/ Suspensão Compatível Astra 1998-2011 Tras</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7893049206266</t>
+          <t>7890903040806</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2062
-Marca: CONTROIL
-Código Produto: C-2062
+          <t>Produto: AMORTECEDOR DE SUSPENSÃO TRASEIRO DIREITO / ESQUERDO NAKATA - HG 30873
+Marca: NAKATA
+Código Produto: HG 30873
 Compatível com os veículos:
-FORD F-1000 L 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
-FORD F-1000 LWB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
-FORD F-4000 - 1984 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 85cv
-FORD F-1000 L 1992 a 1995 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 91cv
-FORD F-4000 - 1993 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
-FORD F-4000 - 1996 a 2008 - Motor: 4 BTAA 8V 3917cc 3.9 L 8V SOHV L4 141cv
-FORD F-1000 4X4 1992 a 1995 - Motor: SERIE 229 3922cc 3.9 L 8V SOHV L4 122cv
-FORD F-1000 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-FORD F-1000 L 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-FORD F-1000 XLT 1996 a 1998 - Motor: HS4 2495cc 2.5 L 8V SOHC L4 116cv
-FORD F-1000 S.CAB 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-FORD F-4000 - 1996 a 1998 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-FORD F-1000 S CAB 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
-FORD F-1000 S.CAB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv</t>
+CHEVROLET ASTRA GLS SFI 16V 1999 a 2006 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
+CHEVROLET ASTRA 2.0 16V 2001 a 2005 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
+CHEVROLET ASTRA 2.0 8V MPFI 1998 a 2003 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
+CHEVROLET ASTRA GL MPFI 2003 a 2004 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
+CHEVROLET ASTRA ADVANTAGE FLEXPOWER SEDAN 2009 a 2011 - Motor: GM FAMILIA II 1998cc 2.0 L 8V SOHC L4 133;140cv
+CHEVROLET ASTRA ELEGANCE MULTIPOWER SFI 1998 a 2006 - Motor: MULTIPOWER 1998cc 2.0 L 8V SOHC L4 106;127cv
+CHEVROLET ASTRA ELEGANCE FLEXPOWER 2004 a 2005 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA ELEGANCE FLEXPOWER 2004 a 2009 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA ELEGANCE FLEXPOWER 2004 a 2010 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA ADVANTAGE FLEXPOWER 2006 a 2006 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA FLEXPOWER SUPER SPORT 2005 a 2009 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA ADVANTAGE FLEXPOWER HATCH 2009 a 2011 - Motor: GM FAMILIA II 1998cc 2.0 L 8V SOHC L4 133;140cv
+CHEVROLET ASTRA ELITE FLEXPOWER 2004 a 2009 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA GL MPFI 8V 1998 a 2005 - Motor: C18NE 1798cc 1.8 L 8V SOHC L4 110;99cv
+CHEVROLET ASTRA FLEXPOWER 2004 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA ADVANTAGE 2004 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA ELEGANCE 2.4 16V 2005 a 2008 - Motor: - 2405cc 2.4 L 16V DOHC L4 147cv
+CHEVROLET ASTRA GL 2007 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA GL MPFI 2001 a 2005 - Motor: C18YE 1798cc 1.8 L 8V SOHC L4 112cv
+CHEVROLET ASTRA 2.0 8V 1998 a 2004 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
+CHEVROLET ASTRA ELEGANCE 2009 a 2011 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA ADVANTAGE FLEXPOWER 2004 a 2008 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA GL MPFI 1999 a 2004 - Motor: C18NE 1798cc 1.8 L 8V SOHC L4 110;99cv
+CHEVROLET ASTRA SPORT MPFI 2000 a 2004 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
+CHEVROLET ASTRA ADVANTAGE FLEXPOWER HATCH AUT. 2009 a 2011 - Motor: GM FAMILIA II 1998cc 2.0 L 8V SOHC L4 133;140cv
+CHEVROLET ASTRA GLS MPFI 1998 a 2006 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
+CHEVROLET ASTRA GLS 2007 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA CONFORT FLEXPOWER 2004 a 2006 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA ELITE FLEXPOWER 2004 a 2009 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA 2.0 16V MPFI 2001 a 2006 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
+CHEVROLET ASTRA ADVANTAGE FLEXPOWER SEDAN AUT. 2009 a 2011 - Motor: GM FAMILIA II 1998cc 2.0 L 8V SOHC L4 133;140cv
+CHEVROLET ASTRA ADVANTAGE FLEXPOWER 2006 a 2010 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA GSI 1999 a 2004 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
+CHEVROLET ASTRA GLS MPFI 1999 a 2005 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
+CHEVROLET ASTRA COMFORT MULTIPOWER SFI 2004 a 2006 - Motor: MULTIPOWER 1998cc 2.0 L 8V SOHC L4 106;127cv
+CHEVROLET ASTRA GLS SFI 16V 1999 a 2003 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
+CHEVROLET ASTRA ADVANTAGE FLEXPOWER 2006 a 2010 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA 2.0 8V MPFI 1998 a 2006 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
+CHEVROLET ASTRA FLEXPOWER 2004 a 2006 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA FLEXPOWER 2004 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA CONFORT FLEXPOWER 2004 a 2008 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA ADVANTAGE 2004 a 2011 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
+CHEVROLET ASTRA CONFORT FLEXPOWER 2004 a 2008 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2062
-Marca: CONTROIL
-Código Produto: C-2062
-Compatível com os veículos:FORD F-4000 (4 BTAA 8V)/(SERIE 10 / X10)/(SERIE 229) 1992-1998 F-1000 2.5 8V/3.9 8V/4.9 12V 1992-1998</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>C-2044</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Cilindro Mestre De Freio Compatível Chevrolet D-20 3.9 8V 1985-1992 Controil C-2044</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Cilindro Mestre De Freio Compatível D-20 3.9 8V 1985-1992</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>7893049204484</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2044
-Marca: CONTROIL
-Código Produto: C-2044
-Compatível com os veículos:
-CHEVROLET BONANZA CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET BONANZA CUSTOM S LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET C-20 4X4 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-CHEVROLET A-20 CUSTOM S 1985 a 1997 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET A-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET D-20 D 20 1985 a 1991 - Motor: Q20B 3871cc 3.9 L 8V SOHC L4 86,4cv
-CHEVROLET A-20 CUSTOM LUXE 1991 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET D-20 CUSTOM LUXE 1991 a 1992 - Motor: Q20B 3871cc 3.9 L 8V SOHC L4 86,4cv
-CHEVROLET A-20 CUSTOM S 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-AGRALE 1800 D 1988 a 1996 - Motor: Q20B 3871cc 3.9 L 8V SOHV L4 86,4cv
-CHEVROLET C-20 STD 1994 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-CHEVROLET A-20 CUSTOM S CAB DUP 1985 a 1996 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET C-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-AGRALE 1800 D 1988 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 88cv
-CHEVROLET D-20 CUSTOM S 1988 a 1991 - Motor: Q20B 3871cc 3.9 L 8V SOHC L4 86,4cv
-CHEVROLET BONANZA CUSTOM S 1989 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET BONANZA CUSTOM S 1989 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET C-20 - 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Produto: CILINDRO MESTRE DE FREIO CONTROIL - C-2044
-Marca: CONTROIL
-Código Produto: C-2044
-Compatível com os veículos:CHEVROLET D-20 3.9 8V 1985-1992 C-20 4.1 12V 1985-1995 BONANZA 4.1 12V 1989-1995 A-20 4.1 12V 1985-1995 AGRALE 1800 (Q20B)/(SERIE 229) 1988-1998</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>C-3308</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Cilindro De Roda Compatível Ford F-4000 (D 226-4) 1979-1983 Direito Controil C-3308</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Cilindro De Roda Compatível F-4000 (D 226-4) 1979-1983 Dir</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>7893049330800</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3308
-Marca: CONTROIL
-Código Produto: C-3308
-Compatível com os veículos:
-AGRALE 1600 A 1986 a 1994 - Motor: - 2470cc 2.5 L 8V SOHC L4 75cv
-AGRALE 1800 D 1988 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 88cv
-AGRALE 1800 D 1988 a 1996 - Motor: Q20B 3871cc 3.9 L 8V SOHV L4 86,4cv
-AGRALE 1600 D 1986 a 1989 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 88cv
-FORD F-400 - 1975 a 1977 - Motor: 272 4457cc 4.5 L 16V OHC V8 165cv
-FORD F-4000 - 1978 a 1986 - Motor: D 226-4 4160cc 4.2 L 8V SOHV L4 86cv
-AGRALE 1600 D 1986 a 1991 - Motor: SERIE 229 2942cc 3.0 L 6V SOHV L3 62cv</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3308
-Marca: CONTROIL
-Código Produto: C-3308
-Compatível com os veículos:FORD F-4000 (D 226-4) 1979-1983 F-400 (272) 1975-1977 AGRALE 1600 (-)/(SERIE 229) 1985-1989 1800 (Q20B)/(SERIE 229) 1988-1989</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Direito</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>C-3334</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Cilindro De Roda Compatível Mercedes Benz L 709 (Om 364) 1988-1996 Controil C-3334</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Cilindro De Roda Compatível Mb L 709 (Om 364) 1988-1996</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>7893049333498</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Produto: CILINDRO DE RODA CONTROIL - C-3334
-Marca: CONTROIL
-Código Produto: C-3334
-Compatível com os veículos:
-MERCEDES BENZ 912 - 1988 a 1996 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 122cv
-MERCEDES BENZ L 709 - 1988 a 1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 90cv
-MERCEDES BENZ L 709 - 1990 a 1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 115cv
-MERCEDES BENZ L 709 37/42 1988 a 1996 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 90cv
-MERCEDES BENZ 710 - 1995 a 1997 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 110cv</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Produto: CILINDRO DE RODA CONTROIL - C-3334
-Marca: CONTROIL
-Código Produto: C-3334
-Compatível com os veículos:MERCEDES BENZ L 709 (OM 364) 1988-1996 912 (OM 364 A) 1988-2003 710 (OM 364 A) 1995-2002</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>C-3377</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Cilindro De Roda Compatível Ford F-1000 3.9 8V 1979-1992 Direito Controil C-3377</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Cilindro De Roda Compatível F-1000 3.9 8V 1979-1992 Dir</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>7893049337717</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3377
-Marca: CONTROIL
-Código Produto: C-3377
-Compatível com os veículos:
-FORD F-1000 L 1981 a 1986 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
-FORD F-1000 L 1979 a 1979 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
-FORD F-1000 L 1979 a 1991 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
-FORD F-1000 L 1980 a 1981 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3377
-Marca: CONTROIL
-Código Produto: C-3377
-Compatível com os veículos:FORD F-1000 3.9 8V 1979-1992</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Direito</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>C-1125</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Reparo Do Cilindro Mestre Compatível Chevrolet D-20 4.0 8V 1993-1996 Controil C-1125</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Reparo Do Cilindro Mestre Compatível D-20 4.0 8V 1993-1996</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>7893049112598</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Produto: REPARO DO CILINDRO MESTRE CONTROIL - C-1125
-Marca: CONTROIL
-Código Produto: C-1125
-Compatível com os veículos:
-CHEVROLET C-20 - 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-CHEVROLET D-20 CUSTOM S TURBO 1992 a 1996 - Motor: S4T 3998cc 4.0 L 8V SOHC L4 120cv
-CHEVROLET VERANEIO LUXE 1993 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET VERANEIO CUSTOM LUXE 1992 a 1993 - Motor: MAXION 3990cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET D-20 CUSTOM LUXE TURBO 1992 a 1996 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-FORD F-4000 - 1984 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 85cv
-CHEVROLET D-20 CHAMP TB 1994 a 1994 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-CHEVROLET D-20 CUSTOM S TURBO 1992 a 1995 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-CHEVROLET D-20 CHAMP 1994 a 1994 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-CHEVROLET C-20 STD 1996 a 1999 - Motor: POWERTECH 4095cc 4.1 L 12V SOHC L6 225cv
-CHEVROLET C-20 4X4 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-CHEVROLET A-20 CUSTOM S 1985 a 1997 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET VERANEIO - 1966 a 1988 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET VERANEIO CUSTOM S 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-FORD F-1000 S CAB 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
-FORD F-4000 - 1993 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
-CHEVROLET A-20 CUSTOM S 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-FORD F-1000 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-CHEVROLET D-20 CUSTOM LUXE TURBO 1996 a 1996 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-CHEVROLET A-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET C-20 CUSTOM LUXE 1996 a 1996 - Motor: POWERTECH 4095cc 4.1 L 12V SOHC L6 225cv
-CHEVROLET C-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-CHEVROLET D-20 LX 1994 a 1998 - Motor: S4T 3998cc 4.0 L 8V SOHC L4 120cv
-CHEVROLET D-20 CUSTOM LUXE 1992 a 1996 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET BONANZA CUSTOM L TB 1992 a 1994 - Motor: S4T 4000cc 4.0 L 8V SOHC L4 120cv
-FORD F-1000 L 1992 a 1995 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 91cv
-FORD F-1000 XLT 1996 a 1998 - Motor: HS4 2495cc 2.5 L 8V SOHC L4 116cv
-CHEVROLET A-20 CUSTOM LUXE 1991 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET D-20 CONQUEST TURBO 1992 a 1995 - Motor: S4T PLUS 3998cc 4.0 L 8V OHV L4 150cv
-FORD F-1000 LWB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
-CHEVROLET BONANZA CUSTOM S 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-FORD F-1000 S.CAB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
-FORD F-1000 S.CAB 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-CHEVROLET BONANZA CUSTOM S 1989 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET BONANZA CUSTOM S TB 1992 a 1995 - Motor: S4T 4000cc 4.0 L 8V SOHC L4 120cv
-CHEVROLET VERANEIO CUSTOM 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET D-20 CONQUEST 1992 a 1994 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET VERANEIO CUSTOM LUXE 1993 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET BONANZA CUSTOM LUXE 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-FORD F-1000 L 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-CHEVROLET VERANEIO - 1983 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-FORD F-4000 - 1996 a 2008 - Motor: 4 BTAA 8V 3917cc 3.9 L 8V SOHV L4 141cv
-CHEVROLET A-20 CUSTOM S CAB DUP 1985 a 1996 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-FORD F-1000 L 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
-CHEVROLET C-20 STD 1994 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-FORD F-4000 - 1996 a 1998 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-FORD F-1000 4X4 1992 a 1995 - Motor: SERIE 229 3922cc 3.9 L 8V SOHV L4 122cv
-CHEVROLET BONANZA CUSTOM S 1989 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET D-20 CUSTOM S 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET BONANZA CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET VERANEIO CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET BONANZA CUSTOM S LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET VERANEIO CUSTOM LUXE 1991 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Produto: REPARO DO CILINDRO MESTRE CONTROIL - C-1125
-Marca: CONTROIL
-Código Produto: C-1125
-Compatível com os veículos:CHEVROLET D-20 4.0 8V 1993-1996 VERANEIO 4.1 12V 1993-1995 C-20 4.1 12V 1993-1996 FORD F-4000 (4 BTAA 8V)/(SERIE 10 / X10)/(SERIE 229) 1992-1998 F-1000 2.5 8V/3.9 8V/4.9 12V 1992-1998</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>C-1478</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Reparo Do Cilindro De Roda Compatível Mercedes Benz L 1519 (Om 355/5) 1973-1987 Controil C-1478</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Reparo Cilindro Roda Compatível Mb L 1519 1973-1987</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>7893049147828</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Produto: REPARO DO CILINDRO DE RODA CONTROIL - C-1478
-Marca: CONTROIL
-Código Produto: C-1478
-Compatível com os veículos:
-MERCEDES BENZ L 1519 - 1972 a 2023 - Motor: OM 355/5 9650cc 9.7 L 10V SOHV L5 192cv</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>Produto: REPARO DO CILINDRO DE RODA CONTROIL - C-1478
-Marca: CONTROIL
-Código Produto: C-1478
-Compatível com os veículos:MERCEDES BENZ L 1519 (OM 355/5) 1973-1987</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
+          <t>Produto: AMORTECEDOR DE SUSPENSÃO TRASEIRO DIREITO / ESQUERDO NAKATA - HG 30873
+Marca: NAKATA
+Código Produto: HG 30873
+Compatível com os veículos:CHEVROLET ASTRA 1.8 8V/2.0 8V/2.4 16V 1998-2011</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>TRASEIRO</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>DIREITO / ESQUERDO</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modified:   anuncios.xlsx modified:   models_excel/core.py modified:   plan.xlsx modified:   view/interface.py
</commit_message>
<xml_diff>
--- a/anuncios.xlsx
+++ b/anuncios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,93 +478,277 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>HG 30873</t>
+          <t>C-3377</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Amortecedor P/ Suspensão Compatível Chevrolet Astra 1.8 8V/2.0 8V/2.4 16V 1998-2011 Traseiro Direito / Esquerdo Nakata Hg 30873</t>
+          <t>Cilindro De Roda Compatível Ford F-1000 3.9 8V 1979-1992 Direito Controil C-3377</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Amortecedor P/ Suspensão Compatível Astra 1998-2011 Tras</t>
+          <t>Cilindro De Roda Compatível F-1000 3.9 8V 1979-1992 Dir</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7890903040806</t>
+          <t>7893049337717</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Produto: AMORTECEDOR DE SUSPENSÃO TRASEIRO DIREITO / ESQUERDO NAKATA - HG 30873
-Marca: NAKATA
-Código Produto: HG 30873
+          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3377
+Marca: CONTROIL
+Código Produto: C-3377
 Compatível com os veículos:
-CHEVROLET ASTRA GLS SFI 16V 1999 a 2006 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
-CHEVROLET ASTRA 2.0 16V 2001 a 2005 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
-CHEVROLET ASTRA 2.0 8V MPFI 1998 a 2003 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
-CHEVROLET ASTRA GL MPFI 2003 a 2004 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
-CHEVROLET ASTRA ADVANTAGE FLEXPOWER SEDAN 2009 a 2011 - Motor: GM FAMILIA II 1998cc 2.0 L 8V SOHC L4 133;140cv
-CHEVROLET ASTRA ELEGANCE MULTIPOWER SFI 1998 a 2006 - Motor: MULTIPOWER 1998cc 2.0 L 8V SOHC L4 106;127cv
-CHEVROLET ASTRA ELEGANCE FLEXPOWER 2004 a 2005 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA ELEGANCE FLEXPOWER 2004 a 2009 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA ELEGANCE FLEXPOWER 2004 a 2010 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA ADVANTAGE FLEXPOWER 2006 a 2006 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA FLEXPOWER SUPER SPORT 2005 a 2009 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA ADVANTAGE FLEXPOWER HATCH 2009 a 2011 - Motor: GM FAMILIA II 1998cc 2.0 L 8V SOHC L4 133;140cv
-CHEVROLET ASTRA ELITE FLEXPOWER 2004 a 2009 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA GL MPFI 8V 1998 a 2005 - Motor: C18NE 1798cc 1.8 L 8V SOHC L4 110;99cv
-CHEVROLET ASTRA FLEXPOWER 2004 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA ADVANTAGE 2004 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA ELEGANCE 2.4 16V 2005 a 2008 - Motor: - 2405cc 2.4 L 16V DOHC L4 147cv
-CHEVROLET ASTRA GL 2007 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA GL MPFI 2001 a 2005 - Motor: C18YE 1798cc 1.8 L 8V SOHC L4 112cv
-CHEVROLET ASTRA 2.0 8V 1998 a 2004 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
-CHEVROLET ASTRA ELEGANCE 2009 a 2011 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA ADVANTAGE FLEXPOWER 2004 a 2008 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA GL MPFI 1999 a 2004 - Motor: C18NE 1798cc 1.8 L 8V SOHC L4 110;99cv
-CHEVROLET ASTRA SPORT MPFI 2000 a 2004 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
-CHEVROLET ASTRA ADVANTAGE FLEXPOWER HATCH AUT. 2009 a 2011 - Motor: GM FAMILIA II 1998cc 2.0 L 8V SOHC L4 133;140cv
-CHEVROLET ASTRA GLS MPFI 1998 a 2006 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
-CHEVROLET ASTRA GLS 2007 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA CONFORT FLEXPOWER 2004 a 2006 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA ELITE FLEXPOWER 2004 a 2009 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA 2.0 16V MPFI 2001 a 2006 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
-CHEVROLET ASTRA ADVANTAGE FLEXPOWER SEDAN AUT. 2009 a 2011 - Motor: GM FAMILIA II 1998cc 2.0 L 8V SOHC L4 133;140cv
-CHEVROLET ASTRA ADVANTAGE FLEXPOWER 2006 a 2010 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA GSI 1999 a 2004 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
-CHEVROLET ASTRA GLS MPFI 1999 a 2005 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
-CHEVROLET ASTRA COMFORT MULTIPOWER SFI 2004 a 2006 - Motor: MULTIPOWER 1998cc 2.0 L 8V SOHC L4 106;127cv
-CHEVROLET ASTRA GLS SFI 16V 1999 a 2003 - Motor: C20SEL 1998cc 2.0 L 16V DOHC L4 136cv
-CHEVROLET ASTRA ADVANTAGE FLEXPOWER 2006 a 2010 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA 2.0 8V MPFI 1998 a 2006 - Motor: C20NE 1998cc 2.0 L 8V SOHC L4 116cv
-CHEVROLET ASTRA FLEXPOWER 2004 a 2006 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA FLEXPOWER 2004 a 2007 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA CONFORT FLEXPOWER 2004 a 2008 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA ADVANTAGE 2004 a 2011 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv
-CHEVROLET ASTRA CONFORT FLEXPOWER 2004 a 2008 - Motor: X20XE 1998cc 2.0 L 8V SOHC L4 121;127cv</t>
+FORD F-1000 L 1981 a 1986 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
+FORD F-1000 L 1979 a 1979 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
+FORD F-1000 L 1979 a 1991 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
+FORD F-1000 L 1980 a 1981 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Produto: AMORTECEDOR DE SUSPENSÃO TRASEIRO DIREITO / ESQUERDO NAKATA - HG 30873
-Marca: NAKATA
-Código Produto: HG 30873
-Compatível com os veículos:CHEVROLET ASTRA 1.8 8V/2.0 8V/2.4 16V 1998-2011</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>TRASEIRO</t>
-        </is>
-      </c>
+          <t>Produto: CILINDRO DE RODA DIREITO CONTROIL - C-3377
+Marca: CONTROIL
+Código Produto: C-3377
+Compatível com os veículos:FORD F-1000 3.9 8V 1979-1992</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>DIREITO / ESQUERDO</t>
-        </is>
-      </c>
+          <t>Direito</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>C-1125</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Reparo Do Cilindro Mestre Compatível Chevrolet D-20 4.0 8V 1993-1996 Controil C-1125</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Reparo Do Cilindro Mestre Compatível D-20 4.0 8V 1993-1996</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>7893049112598</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO CILINDRO MESTRE CONTROIL - C-1125
+Marca: CONTROIL
+Código Produto: C-1125
+Compatível com os veículos:
+CHEVROLET C-20 - 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+CHEVROLET D-20 CUSTOM S TURBO 1992 a 1996 - Motor: S4T 3998cc 4.0 L 8V SOHC L4 120cv
+CHEVROLET VERANEIO LUXE 1993 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET VERANEIO CUSTOM LUXE 1992 a 1993 - Motor: MAXION 3990cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET D-20 CUSTOM LUXE TURBO 1992 a 1996 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+FORD F-4000 - 1984 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 85cv
+CHEVROLET D-20 CHAMP TB 1994 a 1994 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+CHEVROLET D-20 CUSTOM S TURBO 1992 a 1995 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+CHEVROLET D-20 CHAMP 1994 a 1994 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+CHEVROLET C-20 STD 1996 a 1999 - Motor: POWERTECH 4095cc 4.1 L 12V SOHC L6 225cv
+CHEVROLET C-20 4X4 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+CHEVROLET A-20 CUSTOM S 1985 a 1997 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET VERANEIO - 1966 a 1988 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET VERANEIO CUSTOM S 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+FORD F-1000 S CAB 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
+FORD F-4000 - 1993 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
+CHEVROLET A-20 CUSTOM S 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+FORD F-1000 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+CHEVROLET D-20 CUSTOM LUXE TURBO 1996 a 1996 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
+CHEVROLET A-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET C-20 CUSTOM LUXE 1996 a 1996 - Motor: POWERTECH 4095cc 4.1 L 12V SOHC L6 225cv
+CHEVROLET C-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+CHEVROLET D-20 LX 1994 a 1998 - Motor: S4T 3998cc 4.0 L 8V SOHC L4 120cv
+CHEVROLET D-20 CUSTOM LUXE 1992 a 1996 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET BONANZA CUSTOM L TB 1992 a 1994 - Motor: S4T 4000cc 4.0 L 8V SOHC L4 120cv
+FORD F-1000 L 1992 a 1995 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 91cv
+FORD F-1000 XLT 1996 a 1998 - Motor: HS4 2495cc 2.5 L 8V SOHC L4 116cv
+CHEVROLET A-20 CUSTOM LUXE 1991 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET D-20 CONQUEST TURBO 1992 a 1995 - Motor: S4T PLUS 3998cc 4.0 L 8V OHV L4 150cv
+FORD F-1000 LWB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
+CHEVROLET BONANZA CUSTOM S 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+FORD F-1000 S.CAB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
+FORD F-1000 S.CAB 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+CHEVROLET BONANZA CUSTOM S 1989 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET BONANZA CUSTOM S TB 1992 a 1995 - Motor: S4T 4000cc 4.0 L 8V SOHC L4 120cv
+CHEVROLET VERANEIO CUSTOM 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET D-20 CONQUEST 1992 a 1994 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET VERANEIO CUSTOM LUXE 1993 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET BONANZA CUSTOM LUXE 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+FORD F-1000 L 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+CHEVROLET VERANEIO - 1983 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+FORD F-4000 - 1996 a 2008 - Motor: 4 BTAA 8V 3917cc 3.9 L 8V SOHV L4 141cv
+CHEVROLET A-20 CUSTOM S CAB DUP 1985 a 1996 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+FORD F-1000 L 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
+CHEVROLET C-20 STD 1994 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
+FORD F-4000 - 1996 a 1998 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+FORD F-1000 4X4 1992 a 1995 - Motor: SERIE 229 3922cc 3.9 L 8V SOHV L4 122cv
+CHEVROLET BONANZA CUSTOM S 1989 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET D-20 CUSTOM S 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
+CHEVROLET BONANZA CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET VERANEIO CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
+CHEVROLET BONANZA CUSTOM S LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
+CHEVROLET VERANEIO CUSTOM LUXE 1991 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO CILINDRO MESTRE CONTROIL - C-1125
+Marca: CONTROIL
+Código Produto: C-1125
+Compatível com os veículos:CHEVROLET D-20 4.0 8V 1993-1996 VERANEIO 4.1 12V 1993-1995 C-20 4.1 12V 1993-1996 FORD F-4000 (4 BTAA 8V)/(SERIE 10 / X10)/(SERIE 229) 1992-1998 F-1000 2.5 8V/3.9 8V/4.9 12V 1992-1998</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>C-1478</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Reparo Do Cilindro De Roda Compatível Mercedes Benz L 1519 (Om 355/5) 1973-1987 Controil C-1478</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Reparo Cilindro Roda Compatível Mb L 1519 1973-1987</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>7893049147828</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO CILINDRO DE RODA CONTROIL - C-1478
+Marca: CONTROIL
+Código Produto: C-1478
+Compatível com os veículos:
+MERCEDES BENZ L 1519 - 1972 a 2023 - Motor: OM 355/5 9650cc 9.7 L 10V SOHV L5 192cv</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO CILINDRO DE RODA CONTROIL - C-1478
+Marca: CONTROIL
+Código Produto: C-1478
+Compatível com os veículos:MERCEDES BENZ L 1519 (OM 355/5) 1973-1987</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>C-1528</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Reparo Do Pistão Da Pinça Compatível Ford F-4000 (Serie 10 / X10)/(Serie 229) 1985-1998 Controil C-1528</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Reparo Pistão Da Pinça Compatível F-4000 / 1985-1998</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>7893049152822</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO PISTÃO DA PINÇA CONTROIL - C-1528
+Marca: CONTROIL
+Código Produto: C-1528
+Compatível com os veículos:
+FORD F-4000 - 1993 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
+FORD F-4000 - 1996 a 1998 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+AGRALE 1600 A 1986 a 1994 - Motor: - 2470cc 2.5 L 8V SOHC L4 75cv
+FORD F-4000 - 1984 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 85cv
+AGRALE 1800 D 1988 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 88cv
+AGRALE 1800 D 1988 a 1996 - Motor: Q20B 3871cc 3.9 L 8V SOHV L4 86,4cv</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO PISTÃO DA PINÇA CONTROIL - C-1528
+Marca: CONTROIL
+Código Produto: C-1528
+Compatível com os veículos:FORD F-4000 (SERIE 10 / X10)/(SERIE 229) 1985-1998 AGRALE 1800 (Q20B)/(SERIE 229) 1988-1998 1600 (-) 1990-1995</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>C-1526</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Reparo Do Pistão Da Pinça Compatível Mercedes Benz L 1114 (Om 364 La) 1996-2004 Controil C-1526</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Reparo Pistão Da Pinça Compatível Mb L 1114 1996-2004</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>7893049152662</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO PISTÃO DA PINÇA CONTROIL - C-1526
+Marca: CONTROIL
+Código Produto: C-1526
+Compatível com os veículos:
+MERCEDES BENZ 710 - 1995 a 1997 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 110cv
+MERCEDES BENZ L 1114 - 1994 a 2004 - Motor: OM 364 LA 3972cc 4.0 L 8V SOHV L4 136cv
+MERCEDES BENZ 914 - 1994 a 1999 - Motor: OM 364 LA 3972cc 4.0 L 8V SOHV L4 136cv
+MERCEDES BENZ 912 - 1988 a 1996 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 122cv
+MERCEDES BENZ L 709 - 1990 a 1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 115cv
+MERCEDES BENZ L 709 - 1988 a 1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 90cv
+MERCEDES BENZ LB/LO 814 - 1997 a 2002 - Motor: OM 364 LA 3972cc 4.0 L 8V SOHV L4 136cv</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Produto: REPARO DO PISTÃO DA PINÇA CONTROIL - C-1526
+Marca: CONTROIL
+Código Produto: C-1526
+Compatível com os veículos:MERCEDES BENZ L 1114 (OM 364 LA) 1996-2004 LB/LO 814 (OM 364 LA) 1997-2002 914 (OM 364 LA) 1996-2003 912 (OM 364 A) 1989-2003 710 (OM 364 A) 1996-2002</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
modified:   .gitignore modified:   anuncios.xlsx new file:   configs/token.txt new file:   "configs\\token.txt" modified:   models_api/api_max.py modified:   models_excel/core.py modified:   plan.xlsx modified:   teste.py modified:   view/interface.py
</commit_message>
<xml_diff>
--- a/anuncios.xlsx
+++ b/anuncios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,41 @@
           <t>lado</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ncm</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>garantia</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>peso</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>altura embalagem</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>largura embalagem</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>comprimento embalagem</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>qtd por embalagem</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -502,10 +537,23 @@
 Marca: CONTROIL
 Código Produto: C-3377
 Compatível com os veículos:
-FORD F-1000 L 1981 a 1986 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
-FORD F-1000 L 1979 a 1979 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
-FORD F-1000 L 1979 a 1991 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
-FORD F-1000 L 1980 a 1981 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv</t>
+FORD F-1000 L 1979-1992 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
+FORD F-1000 L 1979-1992 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
+FORD F-1000 L 1979-1992 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
+FORD F-1000 L 1979-1992 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 86cv
+Códigos similares:
+ACDELCO: B18E0459
+ORIGINAL OEM: RCCR01259
+BENDIX: 2262058
+FORD ORIGINAL: 85TU/2261/D
+TRW: RCCR01259
+FORD ORIGINAL: 2S4611050
+VARGA: RCCR01259
+BENDIX: 2259800
+ACDELCO: 2259800
+NAKATA: NKF12377
+BOSCH: CR 2058
+ACDELCO: 2262058</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -522,99 +570,106 @@
           <t>Direito</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>87083090</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0,619</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>C-1125</t>
+          <t>HG 41484</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Reparo Do Cilindro Mestre Compatível Chevrolet D-20 4.0 8V 1993-1996 Controil C-1125</t>
+          <t>Amortecedor P/ Suspensão Compatível Fiat Pulse 1.0 12V/1.3 16V/1.3 8V 2021-2025 Dianteiro Esquerdo Nakata Hg 41484</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Reparo Do Cilindro Mestre Compatível D-20 4.0 8V 1993-1996</t>
+          <t>Amortecedor P/ Suspensão Compatível Pulse 1.3 16V/ 2021-2025 Diant Esq</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>7893049112598</t>
+          <t>7890903125732</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Produto: REPARO DO CILINDRO MESTRE CONTROIL - C-1125
-Marca: CONTROIL
-Código Produto: C-1125
+          <t>Produto: AMORTECEDOR DE SUSPENSÃO DIANTEIRO ESQUERDO NAKATA - HG 41484
+Marca: NAKATA
+Código Produto: HG 41484
 Compatível com os veículos:
-CHEVROLET C-20 - 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-CHEVROLET D-20 CUSTOM S TURBO 1992 a 1996 - Motor: S4T 3998cc 4.0 L 8V SOHC L4 120cv
-CHEVROLET VERANEIO LUXE 1993 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET VERANEIO CUSTOM LUXE 1992 a 1993 - Motor: MAXION 3990cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET D-20 CUSTOM LUXE TURBO 1992 a 1996 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-FORD F-4000 - 1984 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 85cv
-CHEVROLET D-20 CHAMP TB 1994 a 1994 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-CHEVROLET D-20 CUSTOM S TURBO 1992 a 1995 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-CHEVROLET D-20 CHAMP 1994 a 1994 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-CHEVROLET C-20 STD 1996 a 1999 - Motor: POWERTECH 4095cc 4.1 L 12V SOHC L6 225cv
-CHEVROLET C-20 4X4 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-CHEVROLET A-20 CUSTOM S 1985 a 1997 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET VERANEIO - 1966 a 1988 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET VERANEIO CUSTOM S 1980 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-FORD F-1000 S CAB 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
-FORD F-4000 - 1993 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
-CHEVROLET A-20 CUSTOM S 1989 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-FORD F-1000 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-CHEVROLET D-20 CUSTOM LUXE TURBO 1996 a 1996 - Motor: S4T PLUS 3998cc 4.0 L 8V SOHC L4 135cv
-CHEVROLET A-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET C-20 CUSTOM LUXE 1996 a 1996 - Motor: POWERTECH 4095cc 4.1 L 12V SOHC L6 225cv
-CHEVROLET C-20 CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-CHEVROLET D-20 LX 1994 a 1998 - Motor: S4T 3998cc 4.0 L 8V SOHC L4 120cv
-CHEVROLET D-20 CUSTOM LUXE 1992 a 1996 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET BONANZA CUSTOM L TB 1992 a 1994 - Motor: S4T 4000cc 4.0 L 8V SOHC L4 120cv
-FORD F-1000 L 1992 a 1995 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 91cv
-FORD F-1000 XLT 1996 a 1998 - Motor: HS4 2495cc 2.5 L 8V SOHC L4 116cv
-CHEVROLET A-20 CUSTOM LUXE 1991 a 1991 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET D-20 CONQUEST TURBO 1992 a 1995 - Motor: S4T PLUS 3998cc 4.0 L 8V OHV L4 150cv
-FORD F-1000 LWB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
-CHEVROLET BONANZA CUSTOM S 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-FORD F-1000 S.CAB 1993 a 1996 - Motor: E-MAX 4913cc 4.9 L 12V SOHC L6 147cv
-FORD F-1000 S.CAB 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-CHEVROLET BONANZA CUSTOM S 1989 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET BONANZA CUSTOM S TB 1992 a 1995 - Motor: S4T 4000cc 4.0 L 8V SOHC L4 120cv
-CHEVROLET VERANEIO CUSTOM 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET D-20 CONQUEST 1992 a 1994 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET VERANEIO CUSTOM LUXE 1993 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET BONANZA CUSTOM LUXE 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-FORD F-1000 L 4X4 1996 a 1999 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-CHEVROLET VERANEIO - 1983 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-FORD F-4000 - 1996 a 2008 - Motor: 4 BTAA 8V 3917cc 3.9 L 8V SOHV L4 141cv
-CHEVROLET A-20 CUSTOM S CAB DUP 1985 a 1996 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-FORD F-1000 L 1996 a 1999 - Motor: E-MAX 4851cc 4.9 L 12V SOHC L6 204cv
-CHEVROLET C-20 STD 1994 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 124cv
-FORD F-4000 - 1996 a 1998 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-FORD F-1000 4X4 1992 a 1995 - Motor: SERIE 229 3922cc 3.9 L 8V SOHV L4 122cv
-CHEVROLET BONANZA CUSTOM S 1989 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET D-20 CUSTOM S 1992 a 1995 - Motor: S4 3998cc 4.0 L 8V SOHC L4 92cv
-CHEVROLET BONANZA CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET VERANEIO CUSTOM LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 121cv
-CHEVROLET BONANZA CUSTOM S LUXE 1991 a 1995 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv
-CHEVROLET VERANEIO CUSTOM LUXE 1991 a 1994 - Motor: 250 4093cc 4.1 L 12V SOHC L6 140cv</t>
+FIAT PULSE IMPETUS 2021-2025 - Motor: GSE 999cc 1.0 L 12V SOHC L3 125;130cv
+FIAT PULSE ABARTH 2022-2025 - Motor: - 1332cc 1.3 L 16V SOHC L4 180;185cv
+FIAT PULSE DRIVE 2021-2025 - Motor: FIREFLY 1332cc 1.3 L 8V SOHC L4 107;98cv
+FIAT PULSE DRIVE 2021-2025 - Motor: GSE 999cc 1.0 L 12V SOHC L3 125;130cv
+FIAT PULSE DRIVE 2021-2025 - Motor: FIREFLY 1332cc 1.3 L 8V SOHC L4 107;98cv
+FIAT PULSE AUDACE 2021-2025 - Motor: GSE 999cc 1.0 L 12V SOHC L3 125;130cv</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Produto: REPARO DO CILINDRO MESTRE CONTROIL - C-1125
-Marca: CONTROIL
-Código Produto: C-1125
-Compatível com os veículos:CHEVROLET D-20 4.0 8V 1993-1996 VERANEIO 4.1 12V 1993-1995 C-20 4.1 12V 1993-1996 FORD F-4000 (4 BTAA 8V)/(SERIE 10 / X10)/(SERIE 229) 1992-1998 F-1000 2.5 8V/3.9 8V/4.9 12V 1992-1998</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+          <t>Produto: AMORTECEDOR DE SUSPENSÃO DIANTEIRO ESQUERDO NAKATA - HG 41484
+Marca: NAKATA
+Código Produto: HG 41484
+Compatível com os veículos:FIAT PULSE 1.0 12V/1.3 16V/1.3 8V 2021-2025</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>DIANTEIRO</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>ESQUERDO</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>87088000</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>3,820</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>170</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>510</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -643,7 +698,14 @@
 Marca: CONTROIL
 Código Produto: C-1478
 Compatível com os veículos:
-MERCEDES BENZ L 1519 - 1972 a 2023 - Motor: OM 355/5 9650cc 9.7 L 10V SOHV L5 192cv</t>
+MERCEDES BENZ L 1519 - 1973-1987 - Motor: OM 355/5 9650cc 9.7 L 10V SOHV L5 192cv
+Códigos similares:
+MERCEDES-BENZ ORIGINAL: 000 586 2342
+TRW: RRCR56564
+ORIGINAL OEM: 2254634
+VARGA: RRCR 5656.4
+ATE: 5140
+BENDIX: 2254634</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -656,6 +718,21 @@
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>87083090</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>0,427</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -684,12 +761,17 @@
 Marca: CONTROIL
 Código Produto: C-1528
 Compatível com os veículos:
-FORD F-4000 - 1993 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
-FORD F-4000 - 1996 a 1998 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
-AGRALE 1600 A 1986 a 1994 - Motor: - 2470cc 2.5 L 8V SOHC L4 75cv
-FORD F-4000 - 1984 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 85cv
-AGRALE 1800 D 1988 a 1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 88cv
-AGRALE 1800 D 1988 a 1996 - Motor: Q20B 3871cc 3.9 L 8V SOHV L4 86,4cv</t>
+FORD F-4000 - 1993-1996 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 87cv
+FORD F-4000 - 1996-1998 - Motor: SERIE 10 / X10 4300cc 4.3 L 8V SOHV L4 135cv
+AGRALE 1600 A 1990-1995 - Motor: - 2470cc 2.5 L 8V SOHC L4 75cv
+FORD F-4000 - 1985-1994 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 85cv
+AGRALE 1800 D 1988-1998 - Motor: SERIE 229 3920cc 3.9 L 8V SOHV L4 88cv
+AGRALE 1800 D 1988-1998 - Motor: Q20B 3871cc 3.9 L 8V SOHV L4 86,4cv
+Códigos similares:
+FORD ORIGINAL: 85HU/2K021/E
+ACDELCO: B18H0263
+VARGA: RRFD 0032.1
+TRW: RRFD00321</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -702,6 +784,21 @@
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>87083090</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>0,071</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -730,13 +827,18 @@
 Marca: CONTROIL
 Código Produto: C-1526
 Compatível com os veículos:
-MERCEDES BENZ 710 - 1995 a 1997 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 110cv
-MERCEDES BENZ L 1114 - 1994 a 2004 - Motor: OM 364 LA 3972cc 4.0 L 8V SOHV L4 136cv
-MERCEDES BENZ 914 - 1994 a 1999 - Motor: OM 364 LA 3972cc 4.0 L 8V SOHV L4 136cv
-MERCEDES BENZ 912 - 1988 a 1996 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 122cv
-MERCEDES BENZ L 709 - 1990 a 1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 115cv
-MERCEDES BENZ L 709 - 1988 a 1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 90cv
-MERCEDES BENZ LB/LO 814 - 1997 a 2002 - Motor: OM 364 LA 3972cc 4.0 L 8V SOHV L4 136cv</t>
+MERCEDES BENZ 710 - 1996-2002 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 110cv
+MERCEDES BENZ L 1114 - 1996-2004 - Motor: OM 364 LA 3972cc 4.0 L 8V SOHV L4 136cv
+MERCEDES BENZ 914 - 1996-2003 - Motor: OM 364 LA 3972cc 4.0 L 8V SOHV L4 136cv
+MERCEDES BENZ 912 - 1989-2003 - Motor: OM 364 A 3972cc 4.0 L 8V SOHV L4 122cv
+MERCEDES BENZ L 709 - 1989-1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 115cv
+MERCEDES BENZ L 709 - 1989-1993 - Motor: OM 364 3972cc 4.0 L 8V SOHV L4 90cv
+MERCEDES BENZ LB/LO 814 - 1997-2002 - Motor: OM 364 LA 3972cc 4.0 L 8V SOHV L4 136cv
+Códigos similares:
+ACDELCO: B18H0262
+MERCEDES-BENZ ORIGINAL: 000.421.6686
+VARGA: RRFD 0044.3
+TRW: RRFD00443</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -749,6 +851,21 @@
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>87083090</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0,070</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>